<commit_message>
Cleaned up, improved fit routines; Python 3 port
All fitting routines are now located within Fitting.py
There should be no need to fidle with it for any general purpose
All necessary parameters can be edited from Plotting_Potato.py
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="0" windowWidth="15300" windowHeight="7660"/>
@@ -24,49 +24,26 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve"> X Thingy</t>
+    <t>Thingy X</t>
   </si>
   <si>
-    <t>Y Thingy</t>
+    <t>Thingy Y</t>
   </si>
   <si>
-    <t>Error  X Thingy</t>
+    <t>Error Thingy X</t>
   </si>
   <si>
-    <t>Error  Y Thingy</t>
+    <t>Error Thingy Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,26 +66,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -413,135 +377,106 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4">
       <c r="A2">
+        <v>-2</v>
+      </c>
+      <c r="B2">
+        <v>-2</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>-1.5</v>
+      </c>
+      <c r="B3">
+        <v>-1.4</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>-1</v>
+      </c>
+      <c r="B4">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>-0.01</v>
+      </c>
+      <c r="C5">
+        <v>0.4</v>
+      </c>
+      <c r="D5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>1.5</v>
+      </c>
+      <c r="B7">
+        <v>1.4</v>
+      </c>
+      <c r="C7">
+        <v>0.6</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>0.15094339622641509</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
-      <c r="A3">
-        <v>2.5</v>
-      </c>
-      <c r="B3">
-        <v>0.30188679245283018</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.49056603773584906</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5">
-        <v>3.5</v>
-      </c>
-      <c r="B5">
-        <v>0.67924528301886788</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0.75471698113207553</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="A7">
-        <v>4.5</v>
-      </c>
-      <c r="B7">
-        <v>0.67924528301886788</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15">
-      <c r="A8">
-        <v>5</v>
-      </c>
       <c r="B8">
-        <v>0.49056603773584906</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9">
-        <v>5.5</v>
-      </c>
-      <c r="B9">
-        <v>0.30188679245283018</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>0.15094339622641509</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.1</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.7</v>
+      </c>
+      <c r="D8">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>